<commit_message>
Refactor BTO management and implement repository functionality
Redesigned `BTORepository` for better handling of projects and exercises, integrating factory methods and error handling. Enhanced `FlatType` with new attributes and updated related classes for improved project management. Added `BTOProjectsView` and updated menu operations for cohesive user interaction. New Excel data files provided for streamlined data handling.
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ExerciseList.xlsx
+++ b/src/main/resources/data/ExerciseList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanchoi/IdeaProjects/SC2002 FCSD Group 2 HDB BTO/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36981D86-479A-674F-902C-20F1DA97AFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECF76D1-8050-B04A-AC99-7766EDC80842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -461,7 +461,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -478,7 +478,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>